<commit_message>
Small changes to project budget
</commit_message>
<xml_diff>
--- a/Project Budget.xlsx
+++ b/Project Budget.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\GitHub\CENG317HardwareProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CBD060C8-3677-461E-8B86-DF3B68B2268B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A708BDED-D60F-4F0D-BC7B-A9A6032E9D9B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12810" xr2:uid="{57D50D5D-4A38-4D21-9B3F-85ADBD554FDF}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
   <si>
     <t>Supplier</t>
   </si>
@@ -124,6 +124,9 @@
   </si>
   <si>
     <t>GRAND TOTAL</t>
+  </si>
+  <si>
+    <t>Kyele Haynes Parts List for CENG317 Hardware Project</t>
   </si>
 </sst>
 </file>
@@ -180,7 +183,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -197,17 +200,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="6" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="6" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="8" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -524,10 +530,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F51DDC9-297F-413D-BA31-CA4CD56178F0}">
-  <dimension ref="A2:G19"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,6 +550,17 @@
     <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+    </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>4</v>
@@ -603,7 +620,7 @@
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="8">
         <v>3538</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -652,19 +669,19 @@
       <c r="A9" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9" s="7">
         <f>SUM(E6:E8)</f>
         <v>142.4974</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -767,7 +784,7 @@
       <c r="A17" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="6">
         <f>SUM(E12:E16)</f>
         <v>136</v>
       </c>
@@ -776,14 +793,15 @@
       <c r="A19" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E19" s="8">
+      <c r="E19" s="7">
         <f>SUM(E9,E17)</f>
         <v>278.49739999999997</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A11:E11"/>
+    <mergeCell ref="A1:G1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G5" r:id="rId1" xr:uid="{8FCFB190-E013-4F78-9A82-2C91ED3DC3D1}"/>

</xml_diff>